<commit_message>
Updated compiled data with latest compression results
</commit_message>
<xml_diff>
--- a/Compiled_Data_Handwritten.xlsx
+++ b/Compiled_Data_Handwritten.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmadi\Desktop\maanas's school stuff\BITS First year\Coding folder\Petasense Project PS1\Compression Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABC712C2-6769-425E-8EB4-8B3AF16616DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5B722-C3F8-41A2-A22A-273F5AF56169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{9DD0B60B-A290-4BDE-A736-38917CBD019E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$H$25</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -162,12 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +507,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,672 +564,673 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C3">
-        <v>73912</v>
+        <v>8350</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D4" si="0">B3/C3</f>
-        <v>0.88667604719125448</v>
+        <f>B3/C3</f>
+        <v>3.1937724550898206</v>
       </c>
       <c r="E3">
-        <v>39710</v>
+        <f>CEILING(B3/F3,1)</f>
+        <v>1680</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F4" si="1">B3/E3</f>
-        <v>1.6503651473180558</v>
+        <v>15.874000000000001</v>
       </c>
       <c r="G3">
-        <v>81460</v>
+        <v>3930</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H4" si="2">B3/G3</f>
-        <v>0.80451755462803831</v>
+        <f>B3/G3</f>
+        <v>6.7857506361323159</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C4">
-        <v>73912</v>
+        <v>8350</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.88667604719125448</v>
+        <f>B4/C4</f>
+        <v>3.1937724550898206</v>
       </c>
       <c r="E4">
-        <v>49043</v>
+        <f t="shared" ref="E4:E25" si="0">CEILING(B4/F4,1)</f>
+        <v>1680</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>1.336296719205595</v>
+        <v>15.874000000000001</v>
       </c>
       <c r="G4">
-        <v>83995</v>
+        <v>3930</v>
       </c>
       <c r="H4">
-        <f t="shared" si="2"/>
-        <v>0.78023691886421809</v>
+        <f>B4/G4</f>
+        <v>6.7857506361323159</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C5">
-        <v>17425</v>
+        <v>19865</v>
       </c>
       <c r="D5">
         <f>B5/C5</f>
-        <v>3.76103299856528</v>
+        <v>1.3424616159073748</v>
       </c>
       <c r="E5">
-        <v>8669</v>
+        <f t="shared" si="0"/>
+        <v>13009</v>
       </c>
       <c r="F5">
-        <f>B5/E5</f>
-        <v>7.5598108201638023</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="G5">
-        <v>16450</v>
+        <v>28560</v>
       </c>
       <c r="H5">
         <f>B5/G5</f>
-        <v>3.9839513677811551</v>
+        <v>0.93375350140056024</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B6">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C6">
-        <v>71371</v>
+        <v>8350</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D25" si="3">B6/C6</f>
-        <v>0.91824410474842721</v>
+        <f>B6/C6</f>
+        <v>3.1937724550898206</v>
       </c>
       <c r="E6">
-        <v>14304</v>
+        <f t="shared" si="0"/>
+        <v>1680</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F25" si="4">B6/E6</f>
-        <v>4.5816554809843399</v>
+        <v>15.874000000000001</v>
       </c>
       <c r="G6">
-        <v>35610</v>
+        <v>3930</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H25" si="5">B6/G6</f>
-        <v>1.8403819151923617</v>
+        <f>B6/G6</f>
+        <v>6.7857506361323159</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B7">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C7">
-        <v>73912</v>
+        <v>8350</v>
       </c>
       <c r="D7">
-        <f t="shared" si="3"/>
-        <v>0.88667604719125448</v>
+        <f>B7/C7</f>
+        <v>3.1937724550898206</v>
       </c>
       <c r="E7">
-        <v>36197</v>
+        <f t="shared" si="0"/>
+        <v>1680</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
-        <v>1.8105367848164213</v>
+        <v>15.874000000000001</v>
       </c>
       <c r="G7">
-        <v>78035</v>
+        <v>3930</v>
       </c>
       <c r="H7">
-        <f t="shared" si="5"/>
-        <v>0.83982828218107264</v>
+        <f>B7/G7</f>
+        <v>6.7857506361323159</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C8">
-        <v>60930</v>
+        <v>16450</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
-        <v>1.0755949450188742</v>
+        <f>B8/C8</f>
+        <v>1.6211550151975684</v>
       </c>
       <c r="E8">
-        <v>7152</v>
+        <f t="shared" si="0"/>
+        <v>8347</v>
       </c>
       <c r="F8">
-        <f t="shared" si="4"/>
-        <v>9.1633109619686799</v>
+        <v>3.1949999999999998</v>
       </c>
       <c r="G8">
-        <v>18600</v>
+        <v>21835</v>
       </c>
       <c r="H8">
-        <f t="shared" si="5"/>
-        <v>3.5234408602150538</v>
+        <f>B8/G8</f>
+        <v>1.2213418822990612</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B9">
-        <v>25600</v>
+        <v>2988</v>
       </c>
       <c r="C9">
-        <v>33940</v>
+        <v>8645</v>
       </c>
       <c r="D9">
-        <f t="shared" si="3"/>
-        <v>0.75427224513847968</v>
+        <f>B9/C9</f>
+        <v>0.3456333140543667</v>
       </c>
       <c r="E9">
-        <v>13357</v>
+        <f t="shared" si="0"/>
+        <v>205</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
-        <v>1.916598038481695</v>
+        <v>14.647</v>
       </c>
       <c r="G9">
-        <v>29840</v>
+        <v>445</v>
       </c>
       <c r="H9">
-        <f t="shared" si="5"/>
-        <v>0.85790884718498661</v>
+        <f>B9/G9</f>
+        <v>6.7146067415730339</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B10">
-        <v>8000</v>
+        <v>2986</v>
       </c>
       <c r="C10">
-        <v>16315</v>
+        <v>8317</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
-        <v>0.49034630707937482</v>
+        <f>B10/C10</f>
+        <v>0.35902368642539378</v>
       </c>
       <c r="E10">
-        <v>3213</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
-        <v>2.4898848428260192</v>
+        <v>14.93</v>
       </c>
       <c r="G10">
-        <v>8445</v>
+        <v>445</v>
       </c>
       <c r="H10">
-        <f t="shared" si="5"/>
-        <v>0.94730609828300771</v>
+        <f>B10/G10</f>
+        <v>6.7101123595505614</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B11">
-        <v>65536</v>
+        <v>2986</v>
       </c>
       <c r="C11">
-        <v>73912</v>
+        <v>8317</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
-        <v>0.88667604719125448</v>
+        <f>B11/C11</f>
+        <v>0.35902368642539378</v>
       </c>
       <c r="E11">
-        <v>62152</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
-        <v>1.0544471617968851</v>
+        <v>14.93</v>
       </c>
       <c r="G11">
-        <v>88105</v>
+        <v>445</v>
       </c>
       <c r="H11">
-        <f t="shared" si="5"/>
-        <v>0.74383973667782755</v>
+        <f>B11/G11</f>
+        <v>6.7101123595505614</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B12">
-        <v>80004</v>
+        <v>17826</v>
       </c>
       <c r="C12">
-        <v>88354</v>
+        <v>23581</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
-        <v>0.90549380899563126</v>
+        <f>B12/C12</f>
+        <v>0.75594758492006275</v>
       </c>
       <c r="E12">
-        <v>109431</v>
+        <f t="shared" si="0"/>
+        <v>21426</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
-        <v>0.73109082435507311</v>
+        <v>0.83199999999999996</v>
       </c>
       <c r="G12">
-        <v>120535</v>
+        <v>17755</v>
       </c>
       <c r="H12">
-        <f t="shared" si="5"/>
-        <v>0.66374082216783503</v>
+        <f>B12/G12</f>
+        <v>1.0039988735567447</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B13">
-        <v>83922</v>
+        <v>17826</v>
       </c>
       <c r="C13">
-        <v>92327</v>
+        <v>23622</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
-        <v>0.90896487484701116</v>
+        <f>B13/C13</f>
+        <v>0.75463550927101852</v>
       </c>
       <c r="E13">
-        <v>121201</v>
+        <f t="shared" si="0"/>
+        <v>21400</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
-        <v>0.69242002953771009</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="G13">
-        <v>128940</v>
+        <v>17710</v>
       </c>
       <c r="H13">
-        <f t="shared" si="5"/>
-        <v>0.65086086551884592</v>
+        <f>B13/G13</f>
+        <v>1.0065499717673632</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B14">
-        <v>26668</v>
+        <v>17826</v>
       </c>
       <c r="C14">
-        <v>8350</v>
+        <v>23601</v>
       </c>
       <c r="D14">
-        <f t="shared" si="3"/>
-        <v>3.1937724550898206</v>
+        <f>B14/C14</f>
+        <v>0.75530697851785944</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>21375</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
-        <v>6667</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="G14">
-        <v>3930</v>
+        <v>17730</v>
       </c>
       <c r="H14">
-        <f t="shared" si="5"/>
-        <v>6.7857506361323159</v>
+        <f>B14/G14</f>
+        <v>1.0054145516074451</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>26668</v>
+        <v>65536</v>
       </c>
       <c r="C15">
-        <v>8350</v>
+        <v>60930</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
-        <v>3.1937724550898206</v>
+        <f>B15/C15</f>
+        <v>1.0755949450188742</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>7158</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
-        <v>6667</v>
+        <v>9.1560000000000006</v>
       </c>
       <c r="G15">
-        <v>3930</v>
+        <v>18600</v>
       </c>
       <c r="H15">
-        <f t="shared" si="5"/>
-        <v>6.7857506361323159</v>
+        <f>B15/G15</f>
+        <v>3.5234408602150538</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>26668</v>
+        <v>25600</v>
       </c>
       <c r="C16">
-        <v>19865</v>
+        <v>33940</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
-        <v>1.3424616159073748</v>
+        <f>B16/C16</f>
+        <v>0.75427224513847968</v>
       </c>
       <c r="E16">
-        <v>13029</v>
+        <f t="shared" si="0"/>
+        <v>13313</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
-        <v>2.0468186353519071</v>
+        <v>1.923</v>
       </c>
       <c r="G16">
-        <v>28560</v>
+        <v>29840</v>
       </c>
       <c r="H16">
-        <f t="shared" si="5"/>
-        <v>0.93375350140056024</v>
+        <f>B16/G16</f>
+        <v>0.85790884718498661</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>26668</v>
+        <v>8000</v>
       </c>
       <c r="C17">
-        <v>8350</v>
+        <v>16315</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
-        <v>3.1937724550898206</v>
+        <f>B17/C17</f>
+        <v>0.49034630707937482</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3213</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
-        <v>6667</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="G17">
-        <v>3930</v>
+        <v>8445</v>
       </c>
       <c r="H17">
-        <f t="shared" si="5"/>
-        <v>6.7857506361323159</v>
+        <f>B17/G17</f>
+        <v>0.94730609828300771</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B18">
-        <v>26668</v>
+        <v>65536</v>
       </c>
       <c r="C18">
-        <v>8350</v>
+        <v>73912</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
-        <v>3.1937724550898206</v>
+        <f>B18/C18</f>
+        <v>0.88667604719125448</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>39623</v>
       </c>
       <c r="F18">
-        <f t="shared" si="4"/>
-        <v>6667</v>
+        <v>1.6539999999999999</v>
       </c>
       <c r="G18">
-        <v>3930</v>
+        <v>81460</v>
       </c>
       <c r="H18">
-        <f t="shared" si="5"/>
-        <v>6.7857506361323159</v>
+        <f>B18/G18</f>
+        <v>0.80451755462803831</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>26668</v>
+        <v>65536</v>
       </c>
       <c r="C19">
-        <v>16450</v>
+        <v>73912</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
-        <v>1.6211550151975684</v>
+        <f>B19/C19</f>
+        <v>0.88667604719125448</v>
       </c>
       <c r="E19">
-        <v>8343</v>
+        <f t="shared" si="0"/>
+        <v>49054</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
-        <v>3.1964521155459669</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="G19">
-        <v>21835</v>
+        <v>83995</v>
       </c>
       <c r="H19">
-        <f t="shared" si="5"/>
-        <v>1.2213418822990612</v>
+        <f>B19/G19</f>
+        <v>0.78023691886421809</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>2988</v>
+        <v>65536</v>
       </c>
       <c r="C20">
-        <v>8645</v>
+        <v>17425</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
-        <v>0.3456333140543667</v>
+        <f>B20/C20</f>
+        <v>3.76103299856528</v>
       </c>
       <c r="E20">
-        <v>195</v>
+        <f t="shared" si="0"/>
+        <v>8675</v>
       </c>
       <c r="F20">
-        <f t="shared" si="4"/>
-        <v>15.323076923076924</v>
+        <v>7.5549999999999997</v>
       </c>
       <c r="G20">
-        <v>445</v>
+        <v>16450</v>
       </c>
       <c r="H20">
-        <f t="shared" si="5"/>
-        <v>6.7146067415730339</v>
+        <f>B20/G20</f>
+        <v>3.9839513677811551</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>2986</v>
+        <v>65536</v>
       </c>
       <c r="C21">
-        <v>8317</v>
+        <v>71371</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
-        <v>0.35902368642539378</v>
+        <f>B21/C21</f>
+        <v>0.91824410474842721</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>14310</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
-        <v>746.5</v>
+        <v>4.58</v>
       </c>
       <c r="G21">
-        <v>445</v>
+        <v>35610</v>
       </c>
       <c r="H21">
-        <f t="shared" si="5"/>
-        <v>6.7101123595505614</v>
+        <f>B21/G21</f>
+        <v>1.8403819151923617</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>2986</v>
+        <v>65536</v>
       </c>
       <c r="C22">
-        <v>8317</v>
+        <v>73912</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
-        <v>0.35902368642539378</v>
+        <f>B22/C22</f>
+        <v>0.88667604719125448</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>36049</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
-        <v>746.5</v>
+        <v>1.8180000000000001</v>
       </c>
       <c r="G22">
-        <v>445</v>
+        <v>78035</v>
       </c>
       <c r="H22">
-        <f t="shared" si="5"/>
-        <v>6.7101123595505614</v>
+        <f>B22/G22</f>
+        <v>0.83982828218107264</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B23">
-        <v>17826</v>
+        <v>65536</v>
       </c>
       <c r="C23">
-        <v>23581</v>
+        <v>73912</v>
       </c>
       <c r="D23">
-        <f t="shared" si="3"/>
-        <v>0.75594758492006275</v>
+        <f>B23/C23</f>
+        <v>0.88667604719125448</v>
       </c>
       <c r="E23">
-        <v>21451</v>
+        <f t="shared" si="0"/>
+        <v>62179</v>
       </c>
       <c r="F23">
-        <f t="shared" si="4"/>
-        <v>0.83101020931425107</v>
+        <v>1.054</v>
       </c>
       <c r="G23">
-        <v>17755</v>
+        <v>88105</v>
       </c>
       <c r="H23">
-        <f t="shared" si="5"/>
-        <v>1.0039988735567447</v>
+        <f>B23/G23</f>
+        <v>0.74383973667782755</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>17826</v>
+        <v>80004</v>
       </c>
       <c r="C24">
-        <v>23622</v>
+        <v>88354</v>
       </c>
       <c r="D24">
-        <f t="shared" si="3"/>
-        <v>0.75463550927101852</v>
+        <f>B24/C24</f>
+        <v>0.90549380899563126</v>
       </c>
       <c r="E24">
-        <v>21427</v>
+        <f t="shared" si="0"/>
+        <v>109445</v>
       </c>
       <c r="F24">
-        <f t="shared" si="4"/>
-        <v>0.83194100900732726</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="G24">
-        <v>17710</v>
+        <v>120535</v>
       </c>
       <c r="H24">
-        <f t="shared" si="5"/>
-        <v>1.0065499717673632</v>
+        <f>B24/G24</f>
+        <v>0.66374082216783503</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B25">
-        <v>17826</v>
+        <v>83922</v>
       </c>
       <c r="C25">
-        <v>23601</v>
+        <v>92327</v>
       </c>
       <c r="D25">
-        <f t="shared" si="3"/>
-        <v>0.75530697851785944</v>
+        <f>B25/C25</f>
+        <v>0.90896487484701116</v>
       </c>
       <c r="E25">
-        <v>21407</v>
+        <f t="shared" si="0"/>
+        <v>120752</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
-        <v>0.83271826972485641</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="G25">
-        <v>17730</v>
+        <v>128940</v>
       </c>
       <c r="H25">
-        <f t="shared" si="5"/>
-        <v>1.0054145516074451</v>
+        <f>B25/G25</f>
+        <v>0.65086086551884592</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:H25" xr:uid="{267054AD-4245-4565-A64A-E80AA23F3A90}"/>
   <mergeCells count="3">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
@@ -1239,35 +1242,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37A473B-D418-424D-9657-E02ED9FD7AC1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451D1EB1-5F13-406E-96D7-6D298D0AB626}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.90625" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="8.6328125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="1.453125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.08984375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1297,672 +1303,677 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C3">
-        <v>73912</v>
+        <v>8350</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D4" si="0">B3/C3</f>
-        <v>0.88667604719125448</v>
+        <f>B3/C3</f>
+        <v>3.1937724550898206</v>
       </c>
       <c r="E3">
-        <v>39710</v>
+        <f>CEILING(B3/F3,1)</f>
+        <v>1680</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F4" si="1">B3/E3</f>
-        <v>1.6503651473180558</v>
+        <v>15.874000000000001</v>
       </c>
       <c r="G3">
-        <v>81460</v>
+        <v>3930</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H4" si="2">B3/G3</f>
-        <v>0.80451755462803831</v>
+        <f>B3/G3</f>
+        <v>6.7857506361323159</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C4">
-        <v>73912</v>
+        <v>8350</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.88667604719125448</v>
+        <f>B4/C4</f>
+        <v>3.1937724550898206</v>
       </c>
       <c r="E4">
-        <v>49043</v>
+        <f>CEILING(B4/F4,1)</f>
+        <v>1680</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>1.336296719205595</v>
+        <v>15.874000000000001</v>
       </c>
       <c r="G4">
-        <v>83995</v>
+        <v>3930</v>
       </c>
       <c r="H4">
-        <f t="shared" si="2"/>
-        <v>0.78023691886421809</v>
+        <f>B4/G4</f>
+        <v>6.7857506361323159</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C5">
-        <v>17425</v>
+        <v>19865</v>
       </c>
       <c r="D5">
         <f>B5/C5</f>
-        <v>3.76103299856528</v>
+        <v>1.3424616159073748</v>
       </c>
       <c r="E5">
-        <v>8669</v>
+        <f>CEILING(B5/F5,1)</f>
+        <v>13009</v>
       </c>
       <c r="F5">
-        <f>B5/E5</f>
-        <v>7.5598108201638023</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="G5">
-        <v>16450</v>
+        <v>28560</v>
       </c>
       <c r="H5">
         <f>B5/G5</f>
-        <v>3.9839513677811551</v>
+        <v>0.93375350140056024</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B6">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C6">
-        <v>71371</v>
+        <v>8350</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D25" si="3">B6/C6</f>
-        <v>0.91824410474842721</v>
+        <f>B6/C6</f>
+        <v>3.1937724550898206</v>
       </c>
       <c r="E6">
-        <v>14304</v>
+        <f>CEILING(B6/F6,1)</f>
+        <v>1680</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F25" si="4">B6/E6</f>
-        <v>4.5816554809843399</v>
+        <v>15.874000000000001</v>
       </c>
       <c r="G6">
-        <v>35610</v>
+        <v>3930</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H25" si="5">B6/G6</f>
-        <v>1.8403819151923617</v>
+        <f>B6/G6</f>
+        <v>6.7857506361323159</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B7">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C7">
-        <v>73912</v>
+        <v>8350</v>
       </c>
       <c r="D7">
-        <f t="shared" si="3"/>
-        <v>0.88667604719125448</v>
+        <f>B7/C7</f>
+        <v>3.1937724550898206</v>
       </c>
       <c r="E7">
-        <v>36197</v>
+        <f>CEILING(B7/F7,1)</f>
+        <v>1680</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
-        <v>1.8105367848164213</v>
+        <v>15.874000000000001</v>
       </c>
       <c r="G7">
-        <v>78035</v>
+        <v>3930</v>
       </c>
       <c r="H7">
-        <f t="shared" si="5"/>
-        <v>0.83982828218107264</v>
+        <f>B7/G7</f>
+        <v>6.7857506361323159</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>65536</v>
+        <v>26668</v>
       </c>
       <c r="C8">
-        <v>60930</v>
+        <v>16450</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
-        <v>1.0755949450188742</v>
+        <f>B8/C8</f>
+        <v>1.6211550151975684</v>
       </c>
       <c r="E8">
-        <v>7152</v>
+        <f>CEILING(B8/F8,1)</f>
+        <v>8347</v>
       </c>
       <c r="F8">
-        <f t="shared" si="4"/>
-        <v>9.1633109619686799</v>
+        <v>3.1949999999999998</v>
       </c>
       <c r="G8">
-        <v>18600</v>
+        <v>21835</v>
       </c>
       <c r="H8">
-        <f t="shared" si="5"/>
-        <v>3.5234408602150538</v>
+        <f>B8/G8</f>
+        <v>1.2213418822990612</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B9">
-        <v>25600</v>
+        <v>2988</v>
       </c>
       <c r="C9">
-        <v>33940</v>
+        <v>8645</v>
       </c>
       <c r="D9">
-        <f t="shared" si="3"/>
-        <v>0.75427224513847968</v>
+        <f>B9/C9</f>
+        <v>0.3456333140543667</v>
       </c>
       <c r="E9">
-        <v>13357</v>
+        <f>CEILING(B9/F9,1)</f>
+        <v>205</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
-        <v>1.916598038481695</v>
+        <v>14.647</v>
       </c>
       <c r="G9">
-        <v>29840</v>
+        <v>445</v>
       </c>
       <c r="H9">
-        <f t="shared" si="5"/>
-        <v>0.85790884718498661</v>
+        <f>B9/G9</f>
+        <v>6.7146067415730339</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B10">
-        <v>8000</v>
+        <v>2986</v>
       </c>
       <c r="C10">
-        <v>16315</v>
+        <v>8317</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
-        <v>0.49034630707937482</v>
+        <f>B10/C10</f>
+        <v>0.35902368642539378</v>
       </c>
       <c r="E10">
-        <v>3213</v>
+        <f>CEILING(B10/F10,1)</f>
+        <v>200</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
-        <v>2.4898848428260192</v>
+        <v>14.93</v>
       </c>
       <c r="G10">
-        <v>8445</v>
+        <v>445</v>
       </c>
       <c r="H10">
-        <f t="shared" si="5"/>
-        <v>0.94730609828300771</v>
+        <f>B10/G10</f>
+        <v>6.7101123595505614</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B11">
-        <v>65536</v>
+        <v>2986</v>
       </c>
       <c r="C11">
-        <v>73912</v>
+        <v>8317</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
-        <v>0.88667604719125448</v>
+        <f>B11/C11</f>
+        <v>0.35902368642539378</v>
       </c>
       <c r="E11">
-        <v>62152</v>
+        <f>CEILING(B11/F11,1)</f>
+        <v>200</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
-        <v>1.0544471617968851</v>
+        <v>14.93</v>
       </c>
       <c r="G11">
-        <v>88105</v>
+        <v>445</v>
       </c>
       <c r="H11">
-        <f t="shared" si="5"/>
-        <v>0.74383973667782755</v>
+        <f>B11/G11</f>
+        <v>6.7101123595505614</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B12">
-        <v>80004</v>
+        <v>17826</v>
       </c>
       <c r="C12">
-        <v>88354</v>
+        <v>23581</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
-        <v>0.90549380899563126</v>
+        <f>B12/C12</f>
+        <v>0.75594758492006275</v>
       </c>
       <c r="E12">
-        <v>109431</v>
+        <f>CEILING(B12/F12,1)</f>
+        <v>21426</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
-        <v>0.73109082435507311</v>
+        <v>0.83199999999999996</v>
       </c>
       <c r="G12">
-        <v>120535</v>
+        <v>17755</v>
       </c>
       <c r="H12">
-        <f t="shared" si="5"/>
-        <v>0.66374082216783503</v>
+        <f>B12/G12</f>
+        <v>1.0039988735567447</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B13">
-        <v>83922</v>
+        <v>17826</v>
       </c>
       <c r="C13">
-        <v>92327</v>
+        <v>23622</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
-        <v>0.90896487484701116</v>
+        <f>B13/C13</f>
+        <v>0.75463550927101852</v>
       </c>
       <c r="E13">
-        <v>121201</v>
+        <f>CEILING(B13/F13,1)</f>
+        <v>21400</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
-        <v>0.69242002953771009</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="G13">
-        <v>128940</v>
+        <v>17710</v>
       </c>
       <c r="H13">
-        <f t="shared" si="5"/>
-        <v>0.65086086551884592</v>
+        <f>B13/G13</f>
+        <v>1.0065499717673632</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B14">
-        <v>26668</v>
+        <v>17826</v>
       </c>
       <c r="C14">
-        <v>8350</v>
+        <v>23601</v>
       </c>
       <c r="D14">
-        <f t="shared" si="3"/>
-        <v>3.1937724550898206</v>
+        <f>B14/C14</f>
+        <v>0.75530697851785944</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <f>CEILING(B14/F14,1)</f>
+        <v>21375</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
-        <v>6667</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="G14">
-        <v>3930</v>
+        <v>17730</v>
       </c>
       <c r="H14">
-        <f t="shared" si="5"/>
-        <v>6.7857506361323159</v>
+        <f>B14/G14</f>
+        <v>1.0054145516074451</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>26668</v>
+        <v>65536</v>
       </c>
       <c r="C15">
-        <v>8350</v>
+        <v>60930</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
-        <v>3.1937724550898206</v>
+        <f>B15/C15</f>
+        <v>1.0755949450188742</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <f>CEILING(B15/F15,1)</f>
+        <v>7158</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
-        <v>6667</v>
+        <v>9.1560000000000006</v>
       </c>
       <c r="G15">
-        <v>3930</v>
+        <v>18600</v>
       </c>
       <c r="H15">
-        <f t="shared" si="5"/>
-        <v>6.7857506361323159</v>
+        <f>B15/G15</f>
+        <v>3.5234408602150538</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>26668</v>
+        <v>25600</v>
       </c>
       <c r="C16">
-        <v>19865</v>
+        <v>33940</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
-        <v>1.3424616159073748</v>
+        <f>B16/C16</f>
+        <v>0.75427224513847968</v>
       </c>
       <c r="E16">
-        <v>13029</v>
+        <f>CEILING(B16/F16,1)</f>
+        <v>13313</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
-        <v>2.0468186353519071</v>
+        <v>1.923</v>
       </c>
       <c r="G16">
-        <v>28560</v>
+        <v>29840</v>
       </c>
       <c r="H16">
-        <f t="shared" si="5"/>
-        <v>0.93375350140056024</v>
+        <f>B16/G16</f>
+        <v>0.85790884718498661</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>26668</v>
+        <v>8000</v>
       </c>
       <c r="C17">
-        <v>8350</v>
+        <v>16315</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
-        <v>3.1937724550898206</v>
+        <f>B17/C17</f>
+        <v>0.49034630707937482</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <f>CEILING(B17/F17,1)</f>
+        <v>3213</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
-        <v>6667</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="G17">
-        <v>3930</v>
+        <v>8445</v>
       </c>
       <c r="H17">
-        <f t="shared" si="5"/>
-        <v>6.7857506361323159</v>
+        <f>B17/G17</f>
+        <v>0.94730609828300771</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B18">
-        <v>26668</v>
+        <v>65536</v>
       </c>
       <c r="C18">
-        <v>8350</v>
+        <v>73912</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
-        <v>3.1937724550898206</v>
+        <f>B18/C18</f>
+        <v>0.88667604719125448</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <f>CEILING(B18/F18,1)</f>
+        <v>39623</v>
       </c>
       <c r="F18">
-        <f t="shared" si="4"/>
-        <v>6667</v>
+        <v>1.6539999999999999</v>
       </c>
       <c r="G18">
-        <v>3930</v>
+        <v>81460</v>
       </c>
       <c r="H18">
-        <f t="shared" si="5"/>
-        <v>6.7857506361323159</v>
+        <f>B18/G18</f>
+        <v>0.80451755462803831</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>26668</v>
+        <v>65536</v>
       </c>
       <c r="C19">
-        <v>16450</v>
+        <v>73912</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
-        <v>1.6211550151975684</v>
+        <f>B19/C19</f>
+        <v>0.88667604719125448</v>
       </c>
       <c r="E19">
-        <v>8343</v>
+        <f>CEILING(B19/F19,1)</f>
+        <v>49054</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
-        <v>3.1964521155459669</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="G19">
-        <v>21835</v>
+        <v>83995</v>
       </c>
       <c r="H19">
-        <f t="shared" si="5"/>
-        <v>1.2213418822990612</v>
+        <f>B19/G19</f>
+        <v>0.78023691886421809</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>2988</v>
+        <v>65536</v>
       </c>
       <c r="C20">
-        <v>8645</v>
+        <v>17425</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
-        <v>0.3456333140543667</v>
+        <f>B20/C20</f>
+        <v>3.76103299856528</v>
       </c>
       <c r="E20">
-        <v>195</v>
+        <f>CEILING(B20/F20,1)</f>
+        <v>8675</v>
       </c>
       <c r="F20">
-        <f t="shared" si="4"/>
-        <v>15.323076923076924</v>
+        <v>7.5549999999999997</v>
       </c>
       <c r="G20">
-        <v>445</v>
+        <v>16450</v>
       </c>
       <c r="H20">
-        <f t="shared" si="5"/>
-        <v>6.7146067415730339</v>
+        <f>B20/G20</f>
+        <v>3.9839513677811551</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>2986</v>
+        <v>65536</v>
       </c>
       <c r="C21">
-        <v>8317</v>
+        <v>71371</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
-        <v>0.35902368642539378</v>
+        <f>B21/C21</f>
+        <v>0.91824410474842721</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <f>CEILING(B21/F21,1)</f>
+        <v>14310</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
-        <v>746.5</v>
+        <v>4.58</v>
       </c>
       <c r="G21">
-        <v>445</v>
+        <v>35610</v>
       </c>
       <c r="H21">
-        <f t="shared" si="5"/>
-        <v>6.7101123595505614</v>
+        <f>B21/G21</f>
+        <v>1.8403819151923617</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>2986</v>
+        <v>65536</v>
       </c>
       <c r="C22">
-        <v>8317</v>
+        <v>73912</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
-        <v>0.35902368642539378</v>
+        <f>B22/C22</f>
+        <v>0.88667604719125448</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <f>CEILING(B22/F22,1)</f>
+        <v>36049</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
-        <v>746.5</v>
+        <v>1.8180000000000001</v>
       </c>
       <c r="G22">
-        <v>445</v>
+        <v>78035</v>
       </c>
       <c r="H22">
-        <f t="shared" si="5"/>
-        <v>6.7101123595505614</v>
+        <f>B22/G22</f>
+        <v>0.83982828218107264</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B23">
-        <v>17826</v>
+        <v>65536</v>
       </c>
       <c r="C23">
-        <v>23581</v>
+        <v>73912</v>
       </c>
       <c r="D23">
-        <f t="shared" si="3"/>
-        <v>0.75594758492006275</v>
+        <f>B23/C23</f>
+        <v>0.88667604719125448</v>
       </c>
       <c r="E23">
-        <v>21451</v>
+        <f>CEILING(B23/F23,1)</f>
+        <v>62179</v>
       </c>
       <c r="F23">
-        <f t="shared" si="4"/>
-        <v>0.83101020931425107</v>
+        <v>1.054</v>
       </c>
       <c r="G23">
-        <v>17755</v>
+        <v>88105</v>
       </c>
       <c r="H23">
-        <f t="shared" si="5"/>
-        <v>1.0039988735567447</v>
+        <f>B23/G23</f>
+        <v>0.74383973667782755</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>17826</v>
+        <v>80004</v>
       </c>
       <c r="C24">
-        <v>23622</v>
+        <v>88354</v>
       </c>
       <c r="D24">
-        <f t="shared" si="3"/>
-        <v>0.75463550927101852</v>
+        <f>B24/C24</f>
+        <v>0.90549380899563126</v>
       </c>
       <c r="E24">
-        <v>21427</v>
+        <f>CEILING(B24/F24,1)</f>
+        <v>109445</v>
       </c>
       <c r="F24">
-        <f t="shared" si="4"/>
-        <v>0.83194100900732726</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="G24">
-        <v>17710</v>
+        <v>120535</v>
       </c>
       <c r="H24">
-        <f t="shared" si="5"/>
-        <v>1.0065499717673632</v>
+        <f>B24/G24</f>
+        <v>0.66374082216783503</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B25">
-        <v>17826</v>
+        <v>83922</v>
       </c>
       <c r="C25">
-        <v>23601</v>
+        <v>92327</v>
       </c>
       <c r="D25">
-        <f t="shared" si="3"/>
-        <v>0.75530697851785944</v>
+        <f>B25/C25</f>
+        <v>0.90896487484701116</v>
       </c>
       <c r="E25">
-        <v>21407</v>
+        <f>CEILING(B25/F25,1)</f>
+        <v>120752</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
-        <v>0.83271826972485641</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="G25">
-        <v>17730</v>
+        <v>128940</v>
       </c>
       <c r="H25">
-        <f t="shared" si="5"/>
-        <v>1.0054145516074451</v>
+        <f>B25/G25</f>
+        <v>0.65086086551884592</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added compiled data in Excel format with compression results
</commit_message>
<xml_diff>
--- a/Compiled_Data_Handwritten.xlsx
+++ b/Compiled_Data_Handwritten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmadi\Desktop\maanas's school stuff\BITS First year\Coding folder\Petasense Project PS1\Compression Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5B722-C3F8-41A2-A22A-273F5AF56169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7F50FD-8EB1-4177-9B5A-8756D51EE0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{9DD0B60B-A290-4BDE-A736-38917CBD019E}"/>
+    <workbookView xWindow="6200" yWindow="630" windowWidth="19200" windowHeight="11170" xr2:uid="{9DD0B60B-A290-4BDE-A736-38917CBD019E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>File Names</t>
   </si>
@@ -130,6 +130,42 @@
   </si>
   <si>
     <t>data3_z.raw</t>
+  </si>
+  <si>
+    <t>data0_ch1.raw</t>
+  </si>
+  <si>
+    <t>data0_ch2.raw</t>
+  </si>
+  <si>
+    <t>data0_ch3.raw</t>
+  </si>
+  <si>
+    <t>data1_ch1.raw</t>
+  </si>
+  <si>
+    <t>data1_ch2.raw</t>
+  </si>
+  <si>
+    <t>data1_ch3.raw</t>
+  </si>
+  <si>
+    <t>data2_ch1.raw</t>
+  </si>
+  <si>
+    <t>data2_ch2.raw</t>
+  </si>
+  <si>
+    <t>data2_ch3.raw</t>
+  </si>
+  <si>
+    <t>data3_ch1.raw</t>
+  </si>
+  <si>
+    <t>data3_ch2.raw</t>
+  </si>
+  <si>
+    <t>data3_ch3.raw</t>
   </si>
 </sst>
 </file>
@@ -165,11 +201,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +544,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G3" sqref="G3:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,350 +601,350 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>26668</v>
       </c>
       <c r="C3">
-        <v>8350</v>
-      </c>
-      <c r="D3">
-        <f>B3/C3</f>
-        <v>3.1937724550898206</v>
+        <f>CEILING(B3/D3,1)</f>
+        <v>19653</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.357</v>
       </c>
       <c r="E3">
         <f>CEILING(B3/F3,1)</f>
-        <v>1680</v>
-      </c>
-      <c r="F3">
-        <v>15.874000000000001</v>
+        <v>12803</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.0830000000000002</v>
       </c>
       <c r="G3">
-        <v>3930</v>
-      </c>
-      <c r="H3">
-        <f>B3/G3</f>
-        <v>6.7857506361323159</v>
+        <f>CEILING(B3/H3,1)</f>
+        <v>28161</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.94699999999999995</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>26668</v>
       </c>
       <c r="C4">
-        <v>8350</v>
-      </c>
-      <c r="D4">
-        <f>B4/C4</f>
-        <v>3.1937724550898206</v>
+        <f t="shared" ref="C4:C25" si="0">CEILING(B4/D4,1)</f>
+        <v>20342</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.3109999999999999</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E25" si="0">CEILING(B4/F4,1)</f>
-        <v>1680</v>
-      </c>
-      <c r="F4">
-        <v>15.874000000000001</v>
+        <f t="shared" ref="E4:E25" si="1">CEILING(B4/F4,1)</f>
+        <v>13719</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.944</v>
       </c>
       <c r="G4">
-        <v>3930</v>
-      </c>
-      <c r="H4">
-        <f>B4/G4</f>
-        <v>6.7857506361323159</v>
+        <f t="shared" ref="G4:G25" si="2">CEILING(B4/H4,1)</f>
+        <v>30032</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.88800000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>26668</v>
       </c>
       <c r="C5">
-        <v>19865</v>
-      </c>
-      <c r="D5">
-        <f>B5/C5</f>
-        <v>1.3424616159073748</v>
+        <f t="shared" si="0"/>
+        <v>19872</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.3420000000000001</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13009</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>2.0499999999999998</v>
       </c>
       <c r="G5">
-        <v>28560</v>
-      </c>
-      <c r="H5">
-        <f>B5/G5</f>
-        <v>0.93375350140056024</v>
+        <f t="shared" si="2"/>
+        <v>28553</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.93400000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>26668</v>
       </c>
       <c r="C6">
-        <v>8350</v>
-      </c>
-      <c r="D6">
-        <f>B6/C6</f>
-        <v>3.1937724550898206</v>
+        <f t="shared" si="0"/>
+        <v>16124</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.6539999999999999</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>1680</v>
-      </c>
-      <c r="F6">
-        <v>15.874000000000001</v>
+        <f t="shared" si="1"/>
+        <v>8077</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3.302</v>
       </c>
       <c r="G6">
-        <v>3930</v>
-      </c>
-      <c r="H6">
-        <f>B6/G6</f>
-        <v>6.7857506361323159</v>
+        <f t="shared" si="2"/>
+        <v>21149</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.2609999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>26668</v>
       </c>
       <c r="C7">
-        <v>8350</v>
-      </c>
-      <c r="D7">
-        <f>B7/C7</f>
-        <v>3.1937724550898206</v>
+        <f t="shared" si="0"/>
+        <v>16954</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.573</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1680</v>
-      </c>
-      <c r="F7">
-        <v>15.874000000000001</v>
+        <f t="shared" si="1"/>
+        <v>9219</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.8929999999999998</v>
       </c>
       <c r="G7">
-        <v>3930</v>
-      </c>
-      <c r="H7">
-        <f>B7/G7</f>
-        <v>6.7857506361323159</v>
+        <f t="shared" si="2"/>
+        <v>23748</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.123</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>26668</v>
       </c>
       <c r="C8">
-        <v>16450</v>
-      </c>
-      <c r="D8">
-        <f>B8/C8</f>
-        <v>1.6211550151975684</v>
+        <f t="shared" si="0"/>
+        <v>16452</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.621</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8347</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>3.1949999999999998</v>
       </c>
       <c r="G8">
-        <v>21835</v>
-      </c>
-      <c r="H8">
-        <f>B8/G8</f>
-        <v>1.2213418822990612</v>
+        <f t="shared" si="2"/>
+        <v>21842</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.2210000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>2988</v>
       </c>
       <c r="C9">
-        <v>8645</v>
-      </c>
-      <c r="D9">
-        <f>B9/C9</f>
-        <v>0.3456333140543667</v>
+        <f t="shared" si="0"/>
+        <v>9829</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.30399999999999999</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>205</v>
-      </c>
-      <c r="F9">
-        <v>14.647</v>
+        <f t="shared" si="1"/>
+        <v>1768</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.6910000000000001</v>
       </c>
       <c r="G9">
-        <v>445</v>
-      </c>
-      <c r="H9">
-        <f>B9/G9</f>
-        <v>6.7146067415730339</v>
+        <f t="shared" si="2"/>
+        <v>3685</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.81100000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>2986</v>
       </c>
       <c r="C10">
-        <v>8317</v>
-      </c>
-      <c r="D10">
-        <f>B10/C10</f>
-        <v>0.35902368642539378</v>
+        <f t="shared" si="0"/>
+        <v>9540</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.313</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="F10">
-        <v>14.93</v>
+        <f t="shared" si="1"/>
+        <v>1753</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.704</v>
       </c>
       <c r="G10">
-        <v>445</v>
-      </c>
-      <c r="H10">
-        <f>B10/G10</f>
-        <v>6.7101123595505614</v>
+        <f t="shared" si="2"/>
+        <v>2986</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>2986</v>
       </c>
       <c r="C11">
-        <v>8317</v>
-      </c>
-      <c r="D11">
-        <f>B11/C11</f>
-        <v>0.35902368642539378</v>
+        <f t="shared" si="0"/>
+        <v>9540</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.313</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="F11">
-        <v>14.93</v>
+        <f t="shared" si="1"/>
+        <v>1778</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.68</v>
       </c>
       <c r="G11">
-        <v>445</v>
-      </c>
-      <c r="H11">
-        <f>B11/G11</f>
-        <v>6.7101123595505614</v>
+        <f t="shared" si="2"/>
+        <v>3701</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.80700000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>17826</v>
       </c>
       <c r="C12">
-        <v>23581</v>
-      </c>
-      <c r="D12">
-        <f>B12/C12</f>
-        <v>0.75594758492006275</v>
+        <f t="shared" si="0"/>
+        <v>23580</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.75600000000000001</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21426</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>0.83199999999999996</v>
       </c>
       <c r="G12">
-        <v>17755</v>
-      </c>
-      <c r="H12">
-        <f>B12/G12</f>
-        <v>1.0039988735567447</v>
+        <f t="shared" si="2"/>
+        <v>17826</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>17826</v>
       </c>
       <c r="C13">
-        <v>23622</v>
-      </c>
-      <c r="D13">
-        <f>B13/C13</f>
-        <v>0.75463550927101852</v>
+        <f t="shared" si="0"/>
+        <v>23611</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.755</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21400</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>0.83299999999999996</v>
       </c>
       <c r="G13">
-        <v>17710</v>
-      </c>
-      <c r="H13">
-        <f>B13/G13</f>
-        <v>1.0065499717673632</v>
+        <f t="shared" si="2"/>
+        <v>17703</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.0069999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>17826</v>
       </c>
       <c r="C14">
-        <v>23601</v>
-      </c>
-      <c r="D14">
-        <f>B14/C14</f>
-        <v>0.75530697851785944</v>
+        <f t="shared" si="0"/>
+        <v>23611</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.755</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21375</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>0.83399999999999996</v>
       </c>
       <c r="G14">
-        <v>17730</v>
-      </c>
-      <c r="H14">
-        <f>B14/G14</f>
-        <v>1.0054145516074451</v>
+        <f t="shared" si="2"/>
+        <v>17738</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.0049999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -918,25 +955,25 @@
         <v>65536</v>
       </c>
       <c r="C15">
-        <v>60930</v>
-      </c>
-      <c r="D15">
-        <f>B15/C15</f>
-        <v>1.0755949450188742</v>
+        <f t="shared" si="0"/>
+        <v>60908</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.0760000000000001</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7158</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>9.1560000000000006</v>
       </c>
       <c r="G15">
-        <v>18600</v>
-      </c>
-      <c r="H15">
-        <f>B15/G15</f>
-        <v>3.5234408602150538</v>
+        <f t="shared" si="2"/>
+        <v>18603</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3.5230000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -947,25 +984,25 @@
         <v>25600</v>
       </c>
       <c r="C16">
-        <v>33940</v>
-      </c>
-      <c r="D16">
-        <f>B16/C16</f>
-        <v>0.75427224513847968</v>
+        <f t="shared" si="0"/>
+        <v>33953</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.754</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13313</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>1.923</v>
       </c>
       <c r="G16">
-        <v>29840</v>
-      </c>
-      <c r="H16">
-        <f>B16/G16</f>
-        <v>0.85790884718498661</v>
+        <f t="shared" si="2"/>
+        <v>29837</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.85799999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -976,25 +1013,25 @@
         <v>8000</v>
       </c>
       <c r="C17">
-        <v>16315</v>
-      </c>
-      <c r="D17">
-        <f>B17/C17</f>
-        <v>0.49034630707937482</v>
+        <f t="shared" si="0"/>
+        <v>16327</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.49</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3213</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>2.4900000000000002</v>
       </c>
       <c r="G17">
-        <v>8445</v>
-      </c>
-      <c r="H17">
-        <f>B17/G17</f>
-        <v>0.94730609828300771</v>
+        <f t="shared" si="2"/>
+        <v>8000</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1005,25 +1042,25 @@
         <v>65536</v>
       </c>
       <c r="C18">
-        <v>73912</v>
-      </c>
-      <c r="D18">
-        <f>B18/C18</f>
-        <v>0.88667604719125448</v>
+        <f t="shared" si="0"/>
+        <v>73886</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.88700000000000001</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39623</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>1.6539999999999999</v>
       </c>
       <c r="G18">
-        <v>81460</v>
-      </c>
-      <c r="H18">
-        <f>B18/G18</f>
-        <v>0.80451755462803831</v>
+        <f t="shared" si="2"/>
+        <v>81412</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.80500000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1034,25 +1071,25 @@
         <v>65536</v>
       </c>
       <c r="C19">
-        <v>73912</v>
-      </c>
-      <c r="D19">
-        <f>B19/C19</f>
-        <v>0.88667604719125448</v>
+        <f t="shared" si="0"/>
+        <v>73886</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.88700000000000001</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49054</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>1.3360000000000001</v>
       </c>
       <c r="G19">
-        <v>83995</v>
-      </c>
-      <c r="H19">
-        <f>B19/G19</f>
-        <v>0.78023691886421809</v>
+        <f t="shared" si="2"/>
+        <v>84021</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.78</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1063,25 +1100,25 @@
         <v>65536</v>
       </c>
       <c r="C20">
-        <v>17425</v>
-      </c>
-      <c r="D20">
-        <f>B20/C20</f>
-        <v>3.76103299856528</v>
+        <f t="shared" si="0"/>
+        <v>17426</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3.7610000000000001</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8675</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>7.5549999999999997</v>
       </c>
       <c r="G20">
+        <f t="shared" si="2"/>
         <v>16450</v>
       </c>
-      <c r="H20">
-        <f>B20/G20</f>
-        <v>3.9839513677811551</v>
+      <c r="H20" s="2">
+        <v>3.984</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1092,25 +1129,25 @@
         <v>65536</v>
       </c>
       <c r="C21">
-        <v>71371</v>
-      </c>
-      <c r="D21">
-        <f>B21/C21</f>
-        <v>0.91824410474842721</v>
+        <f t="shared" si="0"/>
+        <v>71390</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.91800000000000004</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14310</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>4.58</v>
       </c>
       <c r="G21">
-        <v>35610</v>
-      </c>
-      <c r="H21">
-        <f>B21/G21</f>
-        <v>1.8403819151923617</v>
+        <f t="shared" si="2"/>
+        <v>35618</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1.84</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1121,25 +1158,25 @@
         <v>65536</v>
       </c>
       <c r="C22">
-        <v>73912</v>
-      </c>
-      <c r="D22">
-        <f>B22/C22</f>
-        <v>0.88667604719125448</v>
+        <f t="shared" si="0"/>
+        <v>73886</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.88700000000000001</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36049</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>1.8180000000000001</v>
       </c>
       <c r="G22">
-        <v>78035</v>
-      </c>
-      <c r="H22">
-        <f>B22/G22</f>
-        <v>0.83982828218107264</v>
+        <f t="shared" si="2"/>
+        <v>78020</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.84</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1150,25 +1187,25 @@
         <v>65536</v>
       </c>
       <c r="C23">
-        <v>73912</v>
-      </c>
-      <c r="D23">
-        <f>B23/C23</f>
-        <v>0.88667604719125448</v>
+        <f t="shared" si="0"/>
+        <v>73886</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.88700000000000001</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62179</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>1.054</v>
       </c>
       <c r="G23">
-        <v>88105</v>
-      </c>
-      <c r="H23">
-        <f>B23/G23</f>
-        <v>0.74383973667782755</v>
+        <f t="shared" si="2"/>
+        <v>65536</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1179,25 +1216,25 @@
         <v>80004</v>
       </c>
       <c r="C24">
-        <v>88354</v>
-      </c>
-      <c r="D24">
-        <f>B24/C24</f>
-        <v>0.90549380899563126</v>
+        <f t="shared" si="0"/>
+        <v>88403</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.90500000000000003</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>109445</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>0.73099999999999998</v>
       </c>
       <c r="G24">
-        <v>120535</v>
-      </c>
-      <c r="H24">
-        <f>B24/G24</f>
-        <v>0.66374082216783503</v>
+        <f t="shared" si="2"/>
+        <v>120488</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.66400000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1208,25 +1245,25 @@
         <v>83922</v>
       </c>
       <c r="C25">
-        <v>92327</v>
-      </c>
-      <c r="D25">
-        <f>B25/C25</f>
-        <v>0.90896487484701116</v>
+        <f t="shared" si="0"/>
+        <v>92222</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.91</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>120752</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>0.69499999999999995</v>
       </c>
       <c r="G25">
-        <v>128940</v>
-      </c>
-      <c r="H25">
-        <f>B25/G25</f>
-        <v>0.65086086551884592</v>
+        <f t="shared" si="2"/>
+        <v>128913</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.65100000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1312,11 +1349,11 @@
         <v>8350</v>
       </c>
       <c r="D3">
-        <f>B3/C3</f>
+        <f t="shared" ref="D3:D25" si="0">B3/C3</f>
         <v>3.1937724550898206</v>
       </c>
       <c r="E3">
-        <f>CEILING(B3/F3,1)</f>
+        <f t="shared" ref="E3:E25" si="1">CEILING(B3/F3,1)</f>
         <v>1680</v>
       </c>
       <c r="F3">
@@ -1326,7 +1363,7 @@
         <v>3930</v>
       </c>
       <c r="H3">
-        <f>B3/G3</f>
+        <f t="shared" ref="H3:H25" si="2">B3/G3</f>
         <v>6.7857506361323159</v>
       </c>
     </row>
@@ -1341,11 +1378,11 @@
         <v>8350</v>
       </c>
       <c r="D4">
-        <f>B4/C4</f>
+        <f t="shared" si="0"/>
         <v>3.1937724550898206</v>
       </c>
       <c r="E4">
-        <f>CEILING(B4/F4,1)</f>
+        <f t="shared" si="1"/>
         <v>1680</v>
       </c>
       <c r="F4">
@@ -1355,7 +1392,7 @@
         <v>3930</v>
       </c>
       <c r="H4">
-        <f>B4/G4</f>
+        <f t="shared" si="2"/>
         <v>6.7857506361323159</v>
       </c>
     </row>
@@ -1370,11 +1407,11 @@
         <v>19865</v>
       </c>
       <c r="D5">
-        <f>B5/C5</f>
+        <f t="shared" si="0"/>
         <v>1.3424616159073748</v>
       </c>
       <c r="E5">
-        <f>CEILING(B5/F5,1)</f>
+        <f t="shared" si="1"/>
         <v>13009</v>
       </c>
       <c r="F5">
@@ -1384,7 +1421,7 @@
         <v>28560</v>
       </c>
       <c r="H5">
-        <f>B5/G5</f>
+        <f t="shared" si="2"/>
         <v>0.93375350140056024</v>
       </c>
     </row>
@@ -1399,11 +1436,11 @@
         <v>8350</v>
       </c>
       <c r="D6">
-        <f>B6/C6</f>
+        <f t="shared" si="0"/>
         <v>3.1937724550898206</v>
       </c>
       <c r="E6">
-        <f>CEILING(B6/F6,1)</f>
+        <f t="shared" si="1"/>
         <v>1680</v>
       </c>
       <c r="F6">
@@ -1413,7 +1450,7 @@
         <v>3930</v>
       </c>
       <c r="H6">
-        <f>B6/G6</f>
+        <f t="shared" si="2"/>
         <v>6.7857506361323159</v>
       </c>
     </row>
@@ -1428,11 +1465,11 @@
         <v>8350</v>
       </c>
       <c r="D7">
-        <f>B7/C7</f>
+        <f t="shared" si="0"/>
         <v>3.1937724550898206</v>
       </c>
       <c r="E7">
-        <f>CEILING(B7/F7,1)</f>
+        <f t="shared" si="1"/>
         <v>1680</v>
       </c>
       <c r="F7">
@@ -1442,7 +1479,7 @@
         <v>3930</v>
       </c>
       <c r="H7">
-        <f>B7/G7</f>
+        <f t="shared" si="2"/>
         <v>6.7857506361323159</v>
       </c>
     </row>
@@ -1457,11 +1494,11 @@
         <v>16450</v>
       </c>
       <c r="D8">
-        <f>B8/C8</f>
+        <f t="shared" si="0"/>
         <v>1.6211550151975684</v>
       </c>
       <c r="E8">
-        <f>CEILING(B8/F8,1)</f>
+        <f t="shared" si="1"/>
         <v>8347</v>
       </c>
       <c r="F8">
@@ -1471,7 +1508,7 @@
         <v>21835</v>
       </c>
       <c r="H8">
-        <f>B8/G8</f>
+        <f t="shared" si="2"/>
         <v>1.2213418822990612</v>
       </c>
     </row>
@@ -1486,11 +1523,11 @@
         <v>8645</v>
       </c>
       <c r="D9">
-        <f>B9/C9</f>
+        <f t="shared" si="0"/>
         <v>0.3456333140543667</v>
       </c>
       <c r="E9">
-        <f>CEILING(B9/F9,1)</f>
+        <f t="shared" si="1"/>
         <v>205</v>
       </c>
       <c r="F9">
@@ -1500,7 +1537,7 @@
         <v>445</v>
       </c>
       <c r="H9">
-        <f>B9/G9</f>
+        <f t="shared" si="2"/>
         <v>6.7146067415730339</v>
       </c>
     </row>
@@ -1515,11 +1552,11 @@
         <v>8317</v>
       </c>
       <c r="D10">
-        <f>B10/C10</f>
+        <f t="shared" si="0"/>
         <v>0.35902368642539378</v>
       </c>
       <c r="E10">
-        <f>CEILING(B10/F10,1)</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="F10">
@@ -1529,7 +1566,7 @@
         <v>445</v>
       </c>
       <c r="H10">
-        <f>B10/G10</f>
+        <f t="shared" si="2"/>
         <v>6.7101123595505614</v>
       </c>
     </row>
@@ -1544,11 +1581,11 @@
         <v>8317</v>
       </c>
       <c r="D11">
-        <f>B11/C11</f>
+        <f t="shared" si="0"/>
         <v>0.35902368642539378</v>
       </c>
       <c r="E11">
-        <f>CEILING(B11/F11,1)</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="F11">
@@ -1558,7 +1595,7 @@
         <v>445</v>
       </c>
       <c r="H11">
-        <f>B11/G11</f>
+        <f t="shared" si="2"/>
         <v>6.7101123595505614</v>
       </c>
     </row>
@@ -1573,11 +1610,11 @@
         <v>23581</v>
       </c>
       <c r="D12">
-        <f>B12/C12</f>
+        <f t="shared" si="0"/>
         <v>0.75594758492006275</v>
       </c>
       <c r="E12">
-        <f>CEILING(B12/F12,1)</f>
+        <f t="shared" si="1"/>
         <v>21426</v>
       </c>
       <c r="F12">
@@ -1587,7 +1624,7 @@
         <v>17755</v>
       </c>
       <c r="H12">
-        <f>B12/G12</f>
+        <f t="shared" si="2"/>
         <v>1.0039988735567447</v>
       </c>
     </row>
@@ -1602,11 +1639,11 @@
         <v>23622</v>
       </c>
       <c r="D13">
-        <f>B13/C13</f>
+        <f t="shared" si="0"/>
         <v>0.75463550927101852</v>
       </c>
       <c r="E13">
-        <f>CEILING(B13/F13,1)</f>
+        <f t="shared" si="1"/>
         <v>21400</v>
       </c>
       <c r="F13">
@@ -1616,7 +1653,7 @@
         <v>17710</v>
       </c>
       <c r="H13">
-        <f>B13/G13</f>
+        <f t="shared" si="2"/>
         <v>1.0065499717673632</v>
       </c>
     </row>
@@ -1631,11 +1668,11 @@
         <v>23601</v>
       </c>
       <c r="D14">
-        <f>B14/C14</f>
+        <f t="shared" si="0"/>
         <v>0.75530697851785944</v>
       </c>
       <c r="E14">
-        <f>CEILING(B14/F14,1)</f>
+        <f t="shared" si="1"/>
         <v>21375</v>
       </c>
       <c r="F14">
@@ -1645,7 +1682,7 @@
         <v>17730</v>
       </c>
       <c r="H14">
-        <f>B14/G14</f>
+        <f t="shared" si="2"/>
         <v>1.0054145516074451</v>
       </c>
     </row>
@@ -1660,11 +1697,11 @@
         <v>60930</v>
       </c>
       <c r="D15">
-        <f>B15/C15</f>
+        <f t="shared" si="0"/>
         <v>1.0755949450188742</v>
       </c>
       <c r="E15">
-        <f>CEILING(B15/F15,1)</f>
+        <f t="shared" si="1"/>
         <v>7158</v>
       </c>
       <c r="F15">
@@ -1674,7 +1711,7 @@
         <v>18600</v>
       </c>
       <c r="H15">
-        <f>B15/G15</f>
+        <f t="shared" si="2"/>
         <v>3.5234408602150538</v>
       </c>
     </row>
@@ -1689,11 +1726,11 @@
         <v>33940</v>
       </c>
       <c r="D16">
-        <f>B16/C16</f>
+        <f t="shared" si="0"/>
         <v>0.75427224513847968</v>
       </c>
       <c r="E16">
-        <f>CEILING(B16/F16,1)</f>
+        <f t="shared" si="1"/>
         <v>13313</v>
       </c>
       <c r="F16">
@@ -1703,7 +1740,7 @@
         <v>29840</v>
       </c>
       <c r="H16">
-        <f>B16/G16</f>
+        <f t="shared" si="2"/>
         <v>0.85790884718498661</v>
       </c>
     </row>
@@ -1718,11 +1755,11 @@
         <v>16315</v>
       </c>
       <c r="D17">
-        <f>B17/C17</f>
+        <f t="shared" si="0"/>
         <v>0.49034630707937482</v>
       </c>
       <c r="E17">
-        <f>CEILING(B17/F17,1)</f>
+        <f t="shared" si="1"/>
         <v>3213</v>
       </c>
       <c r="F17">
@@ -1732,7 +1769,7 @@
         <v>8445</v>
       </c>
       <c r="H17">
-        <f>B17/G17</f>
+        <f t="shared" si="2"/>
         <v>0.94730609828300771</v>
       </c>
     </row>
@@ -1747,11 +1784,11 @@
         <v>73912</v>
       </c>
       <c r="D18">
-        <f>B18/C18</f>
+        <f t="shared" si="0"/>
         <v>0.88667604719125448</v>
       </c>
       <c r="E18">
-        <f>CEILING(B18/F18,1)</f>
+        <f t="shared" si="1"/>
         <v>39623</v>
       </c>
       <c r="F18">
@@ -1761,7 +1798,7 @@
         <v>81460</v>
       </c>
       <c r="H18">
-        <f>B18/G18</f>
+        <f t="shared" si="2"/>
         <v>0.80451755462803831</v>
       </c>
     </row>
@@ -1776,11 +1813,11 @@
         <v>73912</v>
       </c>
       <c r="D19">
-        <f>B19/C19</f>
+        <f t="shared" si="0"/>
         <v>0.88667604719125448</v>
       </c>
       <c r="E19">
-        <f>CEILING(B19/F19,1)</f>
+        <f t="shared" si="1"/>
         <v>49054</v>
       </c>
       <c r="F19">
@@ -1790,7 +1827,7 @@
         <v>83995</v>
       </c>
       <c r="H19">
-        <f>B19/G19</f>
+        <f t="shared" si="2"/>
         <v>0.78023691886421809</v>
       </c>
     </row>
@@ -1805,11 +1842,11 @@
         <v>17425</v>
       </c>
       <c r="D20">
-        <f>B20/C20</f>
+        <f t="shared" si="0"/>
         <v>3.76103299856528</v>
       </c>
       <c r="E20">
-        <f>CEILING(B20/F20,1)</f>
+        <f t="shared" si="1"/>
         <v>8675</v>
       </c>
       <c r="F20">
@@ -1819,7 +1856,7 @@
         <v>16450</v>
       </c>
       <c r="H20">
-        <f>B20/G20</f>
+        <f t="shared" si="2"/>
         <v>3.9839513677811551</v>
       </c>
     </row>
@@ -1834,11 +1871,11 @@
         <v>71371</v>
       </c>
       <c r="D21">
-        <f>B21/C21</f>
+        <f t="shared" si="0"/>
         <v>0.91824410474842721</v>
       </c>
       <c r="E21">
-        <f>CEILING(B21/F21,1)</f>
+        <f t="shared" si="1"/>
         <v>14310</v>
       </c>
       <c r="F21">
@@ -1848,7 +1885,7 @@
         <v>35610</v>
       </c>
       <c r="H21">
-        <f>B21/G21</f>
+        <f t="shared" si="2"/>
         <v>1.8403819151923617</v>
       </c>
     </row>
@@ -1863,11 +1900,11 @@
         <v>73912</v>
       </c>
       <c r="D22">
-        <f>B22/C22</f>
+        <f t="shared" si="0"/>
         <v>0.88667604719125448</v>
       </c>
       <c r="E22">
-        <f>CEILING(B22/F22,1)</f>
+        <f t="shared" si="1"/>
         <v>36049</v>
       </c>
       <c r="F22">
@@ -1877,7 +1914,7 @@
         <v>78035</v>
       </c>
       <c r="H22">
-        <f>B22/G22</f>
+        <f t="shared" si="2"/>
         <v>0.83982828218107264</v>
       </c>
     </row>
@@ -1892,11 +1929,11 @@
         <v>73912</v>
       </c>
       <c r="D23">
-        <f>B23/C23</f>
+        <f t="shared" si="0"/>
         <v>0.88667604719125448</v>
       </c>
       <c r="E23">
-        <f>CEILING(B23/F23,1)</f>
+        <f t="shared" si="1"/>
         <v>62179</v>
       </c>
       <c r="F23">
@@ -1906,7 +1943,7 @@
         <v>88105</v>
       </c>
       <c r="H23">
-        <f>B23/G23</f>
+        <f t="shared" si="2"/>
         <v>0.74383973667782755</v>
       </c>
     </row>
@@ -1921,11 +1958,11 @@
         <v>88354</v>
       </c>
       <c r="D24">
-        <f>B24/C24</f>
+        <f t="shared" si="0"/>
         <v>0.90549380899563126</v>
       </c>
       <c r="E24">
-        <f>CEILING(B24/F24,1)</f>
+        <f t="shared" si="1"/>
         <v>109445</v>
       </c>
       <c r="F24">
@@ -1935,7 +1972,7 @@
         <v>120535</v>
       </c>
       <c r="H24">
-        <f>B24/G24</f>
+        <f t="shared" si="2"/>
         <v>0.66374082216783503</v>
       </c>
     </row>
@@ -1950,11 +1987,11 @@
         <v>92327</v>
       </c>
       <c r="D25">
-        <f>B25/C25</f>
+        <f t="shared" si="0"/>
         <v>0.90896487484701116</v>
       </c>
       <c r="E25">
-        <f>CEILING(B25/F25,1)</f>
+        <f t="shared" si="1"/>
         <v>120752</v>
       </c>
       <c r="F25">
@@ -1964,7 +2001,7 @@
         <v>128940</v>
       </c>
       <c r="H25">
-        <f>B25/G25</f>
+        <f t="shared" si="2"/>
         <v>0.65086086551884592</v>
       </c>
     </row>

</xml_diff>